<commit_message>
Updated IR_analog.ino to measure 4 sensors at the same time. Took 4 data readings at once, and added them to IRdata.xlsx
</commit_message>
<xml_diff>
--- a/timbot/experiments/irRangeFinders/IRdata.xlsx
+++ b/timbot/experiments/irRangeFinders/IRdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="9555" windowHeight="4695"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="9555" windowHeight="4695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>distance (cm) +- 2mm</t>
   </si>
@@ -28,6 +28,33 @@
   </si>
   <si>
     <t>duplicate data, this is what we might be able to narrow it down to mechanically</t>
+  </si>
+  <si>
+    <t>distance (cm)</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>value black</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>next time: try 45 degree angle</t>
   </si>
 </sst>
 </file>
@@ -339,11 +366,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="172237952"/>
-        <c:axId val="172237376"/>
+        <c:axId val="163853952"/>
+        <c:axId val="163854528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="172237952"/>
+        <c:axId val="163853952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -353,12 +380,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172237376"/>
+        <c:crossAx val="163854528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="172237376"/>
+        <c:axId val="163854528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -369,9 +396,746 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172237952"/>
+        <c:crossAx val="163853952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$8:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$8:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>293</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$8:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$8:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>533</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$8:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$8:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>452</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$8:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$8:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>393</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>454</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>535</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>284</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Average</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$O$8:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>148.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>183.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>208.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>246.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>387.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>449.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>539.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>486.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>295</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="67037184"/>
+        <c:axId val="158166976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="67037184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="158166976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="158166976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67037184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.7082458442694647E-2"/>
+                  <c:y val="0.67068642461358996"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$8:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$O$8:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>148.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>183.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>208.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>246.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>387.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>449.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>539.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="67875840"/>
+        <c:axId val="158170432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="67875840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="158170432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="158170432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67875840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -418,6 +1182,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -715,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -975,24 +1804,470 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>140</v>
+      </c>
+      <c r="C3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>130</v>
+      </c>
+      <c r="C4">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>120</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>110</v>
+      </c>
+      <c r="C6">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>523</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>142</v>
+      </c>
+      <c r="C8">
+        <v>117</v>
+      </c>
+      <c r="D8">
+        <v>201</v>
+      </c>
+      <c r="E8">
+        <v>134</v>
+      </c>
+      <c r="O8">
+        <f>AVERAGE(B8:E8)</f>
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>90</v>
+      </c>
+      <c r="B9">
+        <v>150</v>
+      </c>
+      <c r="C9">
+        <v>146</v>
+      </c>
+      <c r="D9">
+        <v>189</v>
+      </c>
+      <c r="E9">
+        <v>139</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:O20" si="0">AVERAGE(B9:E9)</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>166</v>
+      </c>
+      <c r="C10">
+        <v>164</v>
+      </c>
+      <c r="D10">
+        <v>157</v>
+      </c>
+      <c r="E10">
+        <v>154</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>160.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>70</v>
+      </c>
+      <c r="B11">
+        <v>186</v>
+      </c>
+      <c r="C11">
+        <v>182</v>
+      </c>
+      <c r="D11">
+        <v>185</v>
+      </c>
+      <c r="E11">
+        <v>180</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>183.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>204</v>
+      </c>
+      <c r="C12">
+        <v>209</v>
+      </c>
+      <c r="D12">
+        <v>213</v>
+      </c>
+      <c r="E12">
+        <v>209</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>208.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>240</v>
+      </c>
+      <c r="C13">
+        <v>244</v>
+      </c>
+      <c r="D13">
+        <v>252</v>
+      </c>
+      <c r="E13">
+        <v>251</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>246.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>291</v>
+      </c>
+      <c r="C14">
+        <v>305</v>
+      </c>
+      <c r="D14">
+        <v>307</v>
+      </c>
+      <c r="E14">
+        <v>304</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>301.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>376</v>
+      </c>
+      <c r="C15">
+        <v>392</v>
+      </c>
+      <c r="D15">
+        <v>388</v>
+      </c>
+      <c r="E15">
+        <v>393</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>387.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>448</v>
+      </c>
+      <c r="C16">
+        <v>443</v>
+      </c>
+      <c r="D16">
+        <v>452</v>
+      </c>
+      <c r="E16">
+        <v>454</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>449.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>500</v>
+      </c>
+      <c r="C17">
+        <v>492</v>
+      </c>
+      <c r="D17">
+        <v>505</v>
+      </c>
+      <c r="E17">
+        <v>503</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>544</v>
+      </c>
+      <c r="C18">
+        <v>533</v>
+      </c>
+      <c r="D18">
+        <v>547</v>
+      </c>
+      <c r="E18">
+        <v>535</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>539.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>494</v>
+      </c>
+      <c r="C19">
+        <v>479</v>
+      </c>
+      <c r="D19">
+        <v>504</v>
+      </c>
+      <c r="E19">
+        <v>469</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>486.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>293</v>
+      </c>
+      <c r="C20">
+        <v>302</v>
+      </c>
+      <c r="D20">
+        <v>301</v>
+      </c>
+      <c r="E20">
+        <v>284</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the program to work with 4 rangefinders
</commit_message>
<xml_diff>
--- a/timbot/experiments/irRangeFinders/IRdata.xlsx
+++ b/timbot/experiments/irRangeFinders/IRdata.xlsx
@@ -366,11 +366,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="163853952"/>
-        <c:axId val="163854528"/>
+        <c:axId val="169883264"/>
+        <c:axId val="169883840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="163853952"/>
+        <c:axId val="169883264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,12 +380,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163854528"/>
+        <c:crossAx val="169883840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="163854528"/>
+        <c:axId val="169883840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,14 +396,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163853952"/>
+        <c:crossAx val="169883264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -908,11 +907,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67037184"/>
-        <c:axId val="158166976"/>
+        <c:axId val="168867328"/>
+        <c:axId val="168706048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67037184"/>
+        <c:axId val="168867328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -922,7 +921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158166976"/>
+        <c:crossAx val="168706048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -930,7 +929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158166976"/>
+        <c:axId val="168706048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,7 +940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67037184"/>
+        <c:crossAx val="168867328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1100,11 +1099,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67875840"/>
-        <c:axId val="158170432"/>
+        <c:axId val="168868864"/>
+        <c:axId val="168708352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67875840"/>
+        <c:axId val="168868864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1113,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158170432"/>
+        <c:crossAx val="168708352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1122,7 +1121,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158170432"/>
+        <c:axId val="168708352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,7 +1132,209 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67875840"/>
+        <c:crossAx val="168868864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.0516185476815397E-2"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.62389938757655294"/>
+          <c:h val="0.75791666666666668"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.17654090113735782"/>
+                  <c:y val="-0.42165937591134439"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$O$8:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>148.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>183.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>208.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>246.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>387.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>449.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>539.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$A$8:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="70454784"/>
+        <c:axId val="165649728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="70454784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="165649728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="165649728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70454784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1224,16 +1425,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1247,6 +1448,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1966,7 +2197,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A8" sqref="A8:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated the boxbot code to use the equation we got from excel. unfortunately,the equation is clearly pretty off. we'll have to re-work it.
</commit_message>
<xml_diff>
--- a/timbot/experiments/irRangeFinders/IRdata.xlsx
+++ b/timbot/experiments/irRangeFinders/IRdata.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -366,11 +367,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169883264"/>
-        <c:axId val="169883840"/>
+        <c:axId val="77191936"/>
+        <c:axId val="77191360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169883264"/>
+        <c:axId val="77191936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,12 +381,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169883840"/>
+        <c:crossAx val="77191360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169883840"/>
+        <c:axId val="77191360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,7 +397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169883264"/>
+        <c:crossAx val="77191936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -907,11 +908,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="168867328"/>
-        <c:axId val="168706048"/>
+        <c:axId val="50687488"/>
+        <c:axId val="50620096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="168867328"/>
+        <c:axId val="50687488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +922,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168706048"/>
+        <c:crossAx val="50620096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -929,7 +930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168706048"/>
+        <c:axId val="50620096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +941,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168867328"/>
+        <c:crossAx val="50687488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -996,8 +997,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.7082458442694647E-2"/>
-                  <c:y val="0.67068642461358996"/>
+                  <c:x val="9.8749125109361333E-2"/>
+                  <c:y val="-3.7646908719743369E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1099,11 +1100,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="168868864"/>
-        <c:axId val="168708352"/>
+        <c:axId val="50848768"/>
+        <c:axId val="50622400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="168868864"/>
+        <c:axId val="50848768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168708352"/>
+        <c:crossAx val="50622400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1121,7 +1122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168708352"/>
+        <c:axId val="50622400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168868864"/>
+        <c:crossAx val="50848768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1191,6 +1192,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
+            <c:name>trend</c:name>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
             <c:dispRSqr val="0"/>
@@ -1301,11 +1303,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70454784"/>
-        <c:axId val="165649728"/>
+        <c:axId val="50849280"/>
+        <c:axId val="50624128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70454784"/>
+        <c:axId val="50849280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,7 +1317,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165649728"/>
+        <c:crossAx val="50624128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1323,7 +1325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165649728"/>
+        <c:axId val="50624128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,7 +1336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70454784"/>
+        <c:crossAx val="50849280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1396,15 +1398,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
+      <xdr:colOff>395287</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1425,16 +1427,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1455,16 +1457,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2196,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>